<commit_message>
regs_module_c handle comments corrected
</commit_message>
<xml_diff>
--- a/generator/input/reg_maps/reg_map_briom_2ai.xlsx
+++ b/generator/input/reg_maps/reg_map_briom_2ai.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Hobby\SAND\generator\input\reg_maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14027BCE-54CF-47D2-80A0-B20C110FD011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34564206-F300-4440-934D-99E559E0C56D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="struct_list" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="199">
   <si>
     <t>name</t>
   </si>
@@ -616,9 +616,6 @@
     <t>SAND_PROP_CALLBACK</t>
   </si>
   <si>
-    <t>callback</t>
-  </si>
-  <si>
     <t>only_end</t>
   </si>
   <si>
@@ -628,16 +625,19 @@
     <t>cmd_sand_callback</t>
   </si>
   <si>
-    <t>Temperature addl coeff</t>
-  </si>
-  <si>
     <t>Power voltage mul coeff</t>
   </si>
   <si>
-    <t>Power voltage addl coeff</t>
-  </si>
-  <si>
     <t>Select Vref source (0-Int, 1-Ext)</t>
+  </si>
+  <si>
+    <t>Temperature add coeff</t>
+  </si>
+  <si>
+    <t>Power voltage add coeff</t>
+  </si>
+  <si>
+    <t>(*callback)(void)</t>
   </si>
 </sst>
 </file>
@@ -1155,7 +1155,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L29" sqref="L29"/>
+      <selection pane="bottomRight" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1204,7 +1204,7 @@
       </c>
       <c r="N1" s="14"/>
       <c r="O1" s="17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1245,10 +1245,10 @@
         <v>10</v>
       </c>
       <c r="M2" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>192</v>
       </c>
       <c r="O2" s="17"/>
     </row>
@@ -1493,7 +1493,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M15" sqref="M15:M16"/>
+      <selection pane="bottomRight" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1541,7 +1541,7 @@
       </c>
       <c r="N1" s="14"/>
       <c r="O1" s="17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1582,10 +1582,10 @@
         <v>10</v>
       </c>
       <c r="M2" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>192</v>
       </c>
       <c r="O2" s="17"/>
     </row>
@@ -1605,11 +1605,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M6" sqref="M6"/>
+      <selection pane="bottomRight" activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1657,7 +1657,7 @@
       </c>
       <c r="N1" s="14"/>
       <c r="O1" s="17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1698,10 +1698,10 @@
         <v>10</v>
       </c>
       <c r="M2" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>192</v>
       </c>
       <c r="O2" s="17"/>
     </row>
@@ -1797,10 +1797,10 @@
         <v>6</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="N6" s="7">
-        <v>1</v>
+        <v>193</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -2005,11 +2005,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomRight" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2058,7 +2058,7 @@
       </c>
       <c r="N1" s="14"/>
       <c r="O1" s="17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2099,10 +2099,10 @@
         <v>10</v>
       </c>
       <c r="M2" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>192</v>
       </c>
       <c r="O2" s="17"/>
     </row>
@@ -2383,7 +2383,7 @@
         <v>172</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>44</v>
@@ -2409,7 +2409,7 @@
         <v>173</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>44</v>
@@ -2461,7 +2461,7 @@
         <v>174</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>25</v>
@@ -2508,7 +2508,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O1" sqref="O1:O1048576"/>
+      <selection pane="bottomRight" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2556,7 +2556,7 @@
       </c>
       <c r="N1" s="14"/>
       <c r="O1" s="17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2597,10 +2597,10 @@
         <v>10</v>
       </c>
       <c r="M2" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>192</v>
       </c>
       <c r="O2" s="17"/>
     </row>
@@ -2724,7 +2724,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O1" sqref="O1:O1048576"/>
+      <selection pane="bottomRight" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2772,7 +2772,7 @@
       </c>
       <c r="N1" s="14"/>
       <c r="O1" s="17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2813,10 +2813,10 @@
         <v>10</v>
       </c>
       <c r="M2" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>192</v>
       </c>
       <c r="O2" s="17"/>
     </row>
@@ -3062,7 +3062,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O1" sqref="O1:O1048576"/>
+      <selection pane="bottomRight" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="N1" s="14"/>
       <c r="O1" s="17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3151,10 +3151,10 @@
         <v>10</v>
       </c>
       <c r="M2" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>192</v>
       </c>
       <c r="O2" s="17"/>
     </row>
@@ -3402,7 +3402,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O1" sqref="O1:O1048576"/>
+      <selection pane="bottomRight" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3450,7 +3450,7 @@
       </c>
       <c r="N1" s="14"/>
       <c r="O1" s="17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3491,10 +3491,10 @@
         <v>10</v>
       </c>
       <c r="M2" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>192</v>
       </c>
       <c r="O2" s="17"/>
     </row>
@@ -3630,7 +3630,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O1" sqref="O1:O1048576"/>
+      <selection pane="bottomRight" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3679,7 +3679,7 @@
       </c>
       <c r="N1" s="14"/>
       <c r="O1" s="17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3720,10 +3720,10 @@
         <v>10</v>
       </c>
       <c r="M2" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>192</v>
       </c>
       <c r="O2" s="17"/>
     </row>

</xml_diff>

<commit_message>
ai pseudo buffering algorithm added
</commit_message>
<xml_diff>
--- a/generator/input/reg_maps/reg_map_briom_2ai.xlsx
+++ b/generator/input/reg_maps/reg_map_briom_2ai.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Hobby\SAND\generator\input\reg_maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD850A6D-756A-4EB3-91F2-DBD62F3BDD6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73767659-2F25-47E5-AF7A-5CB213EA395C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="struct_list" sheetId="2" r:id="rId1"/>
@@ -24,12 +24,12 @@
     <sheet name="ai" sheetId="11" r:id="rId9"/>
     <sheet name="test" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="208">
   <si>
     <t>name</t>
   </si>
@@ -641,6 +641,30 @@
   </si>
   <si>
     <t>debug_err_led_on</t>
+  </si>
+  <si>
+    <t>meas_calib_b</t>
+  </si>
+  <si>
+    <t>meas_calib_a</t>
+  </si>
+  <si>
+    <t>meas_value</t>
+  </si>
+  <si>
+    <t>Engineer units value</t>
+  </si>
+  <si>
+    <t>Engineer units add</t>
+  </si>
+  <si>
+    <t>Engineer units mul</t>
+  </si>
+  <si>
+    <t>{1.0f,1.0f}</t>
+  </si>
+  <si>
+    <t>avg_num</t>
   </si>
 </sst>
 </file>
@@ -1091,7 +1115,7 @@
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1154,7 +1178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52FF13CE-6448-41FA-BA7B-6B713DD2EE28}">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -3639,13 +3663,13 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{622EF646-023E-42FD-8335-9337B02D684D}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M2" sqref="M2"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3854,6 +3878,107 @@
         <v>1014</v>
       </c>
     </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="7">
+        <v>2</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="F8" s="8">
+        <v>1018</v>
+      </c>
+      <c r="G8" s="9">
+        <v>10</v>
+      </c>
+      <c r="H8" s="9">
+        <v>1</v>
+      </c>
+      <c r="I8" s="9">
+        <v>100</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="7">
+        <v>2</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="8">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="7">
+        <v>2</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="F10" s="8">
+        <v>1024</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="7">
+        <v>2</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="F11" s="8">
+        <v>1028</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:E1"/>

</xml_diff>

<commit_message>
select adc_int vref by register
</commit_message>
<xml_diff>
--- a/generator/input/reg_maps/reg_map_briom_2ai.xlsx
+++ b/generator/input/reg_maps/reg_map_briom_2ai.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Hobby\SAND\generator\input\reg_maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73767659-2F25-47E5-AF7A-5CB213EA395C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE2B740-9DE3-4A4A-A328-9E1FA023B672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="struct_list" sheetId="2" r:id="rId1"/>
@@ -2044,11 +2044,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M2" sqref="M2"/>
+      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2515,7 +2515,7 @@
         <v>386</v>
       </c>
       <c r="G19" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" s="9">
         <v>0</v>
@@ -3665,7 +3665,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{622EF646-023E-42FD-8335-9337B02D684D}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>

</xml_diff>

<commit_message>
select ai vref by register
</commit_message>
<xml_diff>
--- a/generator/input/reg_maps/reg_map_briom_2ai.xlsx
+++ b/generator/input/reg_maps/reg_map_briom_2ai.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Hobby\SAND\generator\input\reg_maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE2B740-9DE3-4A4A-A328-9E1FA023B672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99CB5B89-7D43-440F-9607-C88425651D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="struct_list" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="210">
   <si>
     <t>name</t>
   </si>
@@ -665,6 +665,12 @@
   </si>
   <si>
     <t>avg_num</t>
+  </si>
+  <si>
+    <t>Samples number for average</t>
+  </si>
+  <si>
+    <t>ai_vref_sel</t>
   </si>
 </sst>
 </file>
@@ -2044,11 +2050,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
+      <selection pane="bottomRight" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3663,10 +3669,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{622EF646-023E-42FD-8335-9337B02D684D}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="5" ySplit="2" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
@@ -3675,7 +3681,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.28515625" style="7" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
@@ -3882,6 +3888,9 @@
       <c r="A8" s="7" t="s">
         <v>207</v>
       </c>
+      <c r="B8" s="7" t="s">
+        <v>208</v>
+      </c>
       <c r="C8" s="7" t="s">
         <v>25</v>
       </c>
@@ -3976,6 +3985,38 @@
         <v>206</v>
       </c>
       <c r="J11" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="7">
+        <v>1</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="F12" s="8">
+        <v>1032</v>
+      </c>
+      <c r="G12" s="9">
+        <v>1</v>
+      </c>
+      <c r="H12" s="9">
+        <v>0</v>
+      </c>
+      <c r="I12" s="9">
+        <v>1</v>
+      </c>
+      <c r="J12" s="10" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>